<commit_message>
week 3 huvec control
</commit_message>
<xml_diff>
--- a/rad_pipeline/week_two_cells_layout.xlsx
+++ b/rad_pipeline/week_two_cells_layout.xlsx
@@ -94,172 +94,172 @@
     <t>r08c12</t>
   </si>
   <si>
+    <t>r01c04</t>
+  </si>
+  <si>
+    <t>Compound_1</t>
+  </si>
+  <si>
+    <t>r01c05</t>
+  </si>
+  <si>
+    <t>Compound_9</t>
+  </si>
+  <si>
+    <t>r01c06</t>
+  </si>
+  <si>
+    <t>Compound_17</t>
+  </si>
+  <si>
+    <t>r02c04</t>
+  </si>
+  <si>
+    <t>Compound_2</t>
+  </si>
+  <si>
+    <t>r02c05</t>
+  </si>
+  <si>
+    <t>Compound_10</t>
+  </si>
+  <si>
+    <t>untreated</t>
+  </si>
+  <si>
+    <t>r03c04</t>
+  </si>
+  <si>
+    <t>Compound_3</t>
+  </si>
+  <si>
+    <t>r03c05</t>
+  </si>
+  <si>
+    <t>Compound_11</t>
+  </si>
+  <si>
+    <t>r03c06</t>
+  </si>
+  <si>
+    <t>r04c04</t>
+  </si>
+  <si>
+    <t>Compound_4</t>
+  </si>
+  <si>
+    <t>r04c05</t>
+  </si>
+  <si>
+    <t>Compound_12</t>
+  </si>
+  <si>
+    <t>r05c04</t>
+  </si>
+  <si>
+    <t>Compound_5</t>
+  </si>
+  <si>
+    <t>r05c05</t>
+  </si>
+  <si>
+    <t>Compound_13</t>
+  </si>
+  <si>
+    <t>r05c06</t>
+  </si>
+  <si>
+    <t>r06c04</t>
+  </si>
+  <si>
+    <t>Compound_6</t>
+  </si>
+  <si>
+    <t>r06c05</t>
+  </si>
+  <si>
+    <t>Compound_14</t>
+  </si>
+  <si>
+    <t>r06c06</t>
+  </si>
+  <si>
+    <t>Compound_7</t>
+  </si>
+  <si>
+    <t>r07c05</t>
+  </si>
+  <si>
+    <t>Compound_15</t>
+  </si>
+  <si>
+    <t>r07c06</t>
+  </si>
+  <si>
+    <t>r08c04</t>
+  </si>
+  <si>
+    <t>Compound_8</t>
+  </si>
+  <si>
+    <t>r08c05</t>
+  </si>
+  <si>
+    <t>Compound_16</t>
+  </si>
+  <si>
+    <t>r08c06</t>
+  </si>
+  <si>
     <t>r01c01</t>
   </si>
   <si>
-    <t>Compound_1</t>
-  </si>
-  <si>
-    <t>Compound_9</t>
-  </si>
-  <si>
     <t>r01c03</t>
   </si>
   <si>
-    <t>Compound_17</t>
-  </si>
-  <si>
-    <t>Compound_2</t>
-  </si>
-  <si>
     <t>r02c02</t>
   </si>
   <si>
-    <t>Compound_10</t>
-  </si>
-  <si>
     <t>r02c03</t>
   </si>
   <si>
-    <t>untreated</t>
-  </si>
-  <si>
     <t>r03c01</t>
   </si>
   <si>
-    <t>Compound_3</t>
-  </si>
-  <si>
-    <t>Compound_11</t>
-  </si>
-  <si>
     <t>r03c03</t>
   </si>
   <si>
-    <t>Compound_4</t>
-  </si>
-  <si>
     <t>r04c02</t>
   </si>
   <si>
-    <t>Compound_12</t>
-  </si>
-  <si>
     <t>r04c03</t>
   </si>
   <si>
     <t>r05c01</t>
   </si>
   <si>
-    <t>Compound_5</t>
-  </si>
-  <si>
     <t>r05c02</t>
   </si>
   <si>
-    <t>Compound_13</t>
-  </si>
-  <si>
     <t>r05c03</t>
   </si>
   <si>
     <t>r06c01</t>
   </si>
   <si>
-    <t>Compound_6</t>
-  </si>
-  <si>
     <t>r06c02</t>
   </si>
   <si>
-    <t>Compound_14</t>
-  </si>
-  <si>
     <t>r06c03</t>
   </si>
   <si>
     <t>r07c01</t>
   </si>
   <si>
-    <t>Compound_7</t>
-  </si>
-  <si>
-    <t>Compound_15</t>
-  </si>
-  <si>
     <t>r07c03</t>
   </si>
   <si>
-    <t>Compound_8</t>
-  </si>
-  <si>
     <t>r08c02</t>
-  </si>
-  <si>
-    <t>Compound_16</t>
-  </si>
-  <si>
-    <t>r01c04</t>
-  </si>
-  <si>
-    <t>r01c05</t>
-  </si>
-  <si>
-    <t>r01c06</t>
-  </si>
-  <si>
-    <t>r02c04</t>
-  </si>
-  <si>
-    <t>r02c05</t>
-  </si>
-  <si>
-    <t>r03c04</t>
-  </si>
-  <si>
-    <t>r03c05</t>
-  </si>
-  <si>
-    <t>r03c06</t>
-  </si>
-  <si>
-    <t>r04c04</t>
-  </si>
-  <si>
-    <t>r04c05</t>
-  </si>
-  <si>
-    <t>r05c04</t>
-  </si>
-  <si>
-    <t>r05c05</t>
-  </si>
-  <si>
-    <t>r05c06</t>
-  </si>
-  <si>
-    <t>r06c04</t>
-  </si>
-  <si>
-    <t>r06c05</t>
-  </si>
-  <si>
-    <t>r06c06</t>
-  </si>
-  <si>
-    <t>r07c05</t>
-  </si>
-  <si>
-    <t>r07c06</t>
-  </si>
-  <si>
-    <t>r08c04</t>
-  </si>
-  <si>
-    <t>r08c05</t>
-  </si>
-  <si>
-    <t>r08c06</t>
   </si>
 </sst>
 </file>
@@ -2874,7 +2874,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="12.63"/>
+    <col customWidth="1" min="1" max="2" width="12.63"/>
+    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2886,7 +2887,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2894,191 +2895,193 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
+      <c r="A4" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
+      <c r="A5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>32</v>
+      <c r="A6" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
+      <c r="A7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
+      <c r="A11" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
+      <c r="A12" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>43</v>
+      <c r="A13" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>44</v>
+      <c r="A14" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>46</v>
+      <c r="A15" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>48</v>
+      <c r="A16" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>49</v>
+      <c r="A17" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>51</v>
+      <c r="A18" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>53</v>
+      <c r="A19" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>54</v>
+      <c r="A20" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>14</v>
+      <c r="A21" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>57</v>
+      <c r="A22" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>16</v>
+      <c r="A23" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>59</v>
+      <c r="A24" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>17</v>
+      <c r="A25" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="1"/>
+    </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>
@@ -3099,15 +3102,12 @@
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="1"/>
       <c r="B47" s="3"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
     <row r="50" ht="15.75" customHeight="1"/>
@@ -4088,200 +4088,199 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>61</v>
+      <c r="A2" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>62</v>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>81</v>
+      <c r="A25" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1"/>
       <c r="B27" s="3"/>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
@@ -4303,9 +4302,15 @@
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="1"/>
+    </row>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
     <row r="52" ht="15.75" customHeight="1"/>

</xml_diff>